<commit_message>
Added noe total xcel spreadsheet
</commit_message>
<xml_diff>
--- a/projects/TrpLoop2b/noe_total.xlsx
+++ b/projects/TrpLoop2b/noe_total.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="20" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
@@ -10,7 +10,7 @@
     <sheet name="TrpLoop2a_NOE" sheetId="1" r:id="rId1"/>
     <sheet name="TrpLoop2b_NOE" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="225">
   <si>
     <t>I</t>
   </si>
@@ -692,6 +692,9 @@
   </si>
   <si>
     <t>r^-6</t>
+  </si>
+  <si>
+    <t>&lt;r^-6&gt;^-1/6 (nm)</t>
   </si>
 </sst>
 </file>
@@ -744,8 +747,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="365">
+  <cellStyleXfs count="367">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1117,7 +1122,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="365">
+  <cellStyles count="367">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1300,6 +1305,7 @@
     <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1482,6 +1488,7 @@
     <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1905,11 +1912,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2122938344"/>
-        <c:axId val="2122949016"/>
+        <c:axId val="-2084737800"/>
+        <c:axId val="-2076714792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2122938344"/>
+        <c:axId val="-2084737800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20000.0"/>
@@ -1967,12 +1974,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2122949016"/>
+        <c:crossAx val="-2076714792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2122949016"/>
+        <c:axId val="-2076714792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2029,7 +2036,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2122938344"/>
+        <c:crossAx val="-2084737800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3418,11 +3425,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2122138376"/>
-        <c:axId val="2122156024"/>
+        <c:axId val="-2087604312"/>
+        <c:axId val="-2122438904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2122138376"/>
+        <c:axId val="-2087604312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20000.0"/>
@@ -3480,12 +3487,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2122156024"/>
+        <c:crossAx val="-2122438904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2122156024"/>
+        <c:axId val="-2122438904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3542,7 +3549,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2122138376"/>
+        <c:crossAx val="-2087604312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5028,7 +5035,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5749,12 +5756,13 @@
   <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -5764,6 +5772,9 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
@@ -5776,6 +5787,10 @@
         <v>4017402</v>
       </c>
       <c r="D2" s="1"/>
+      <c r="E2">
+        <f>B2^(-1/6)</f>
+        <v>0.24728296497342106</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
@@ -5790,6 +5805,10 @@
         <v>1375662</v>
       </c>
       <c r="D3" s="1"/>
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="0">B3^(-1/6)</f>
+        <v>0.28520229366604805</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
@@ -5804,6 +5823,10 @@
         <v>11779189</v>
       </c>
       <c r="D4" s="1"/>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.56493318280525495</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
@@ -5818,6 +5841,10 @@
         <v>5479610</v>
       </c>
       <c r="D5" s="1"/>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.78543555762584205</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
@@ -5832,6 +5859,10 @@
         <v>33159142</v>
       </c>
       <c r="D6" s="1"/>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.13470728759360401</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
@@ -5846,6 +5877,10 @@
         <v>942996</v>
       </c>
       <c r="D7" s="1"/>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.84479373734229002</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
@@ -5860,6 +5895,10 @@
         <v>4604326</v>
       </c>
       <c r="D8" s="1"/>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.61897826277954315</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
@@ -5874,6 +5913,10 @@
         <v>1929442</v>
       </c>
       <c r="D9" s="1"/>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.40968361513580703</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
@@ -5888,6 +5931,10 @@
         <v>4105617</v>
       </c>
       <c r="D10" s="1"/>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.51283812422702102</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
@@ -5902,6 +5949,10 @@
         <v>14260496</v>
       </c>
       <c r="D11" s="1"/>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.22901919488493802</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
@@ -5913,6 +5964,10 @@
         <v>14260496</v>
       </c>
       <c r="D12" s="1"/>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.48191142100420797</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
@@ -5927,6 +5982,10 @@
         <v>3495684</v>
       </c>
       <c r="D13" s="1"/>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.67498213444495403</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
@@ -5938,6 +5997,10 @@
         <v>3495684</v>
       </c>
       <c r="D14" s="1"/>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.28653207520784507</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
@@ -5952,6 +6015,10 @@
         <v>4070468</v>
       </c>
       <c r="D15" s="1"/>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.55167406544247199</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
@@ -5966,6 +6033,10 @@
         <v>1688172</v>
       </c>
       <c r="D16" s="1"/>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.23980711264928703</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
@@ -5980,6 +6051,10 @@
         <v>767850</v>
       </c>
       <c r="D17" s="1"/>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.278061567071126</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
@@ -5994,6 +6069,10 @@
         <v>21454114</v>
       </c>
       <c r="D18" s="1"/>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0.22878703451428206</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
@@ -6008,6 +6087,10 @@
         <v>10431032</v>
       </c>
       <c r="D19" s="1"/>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0.29902750215706803</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
@@ -6022,6 +6105,10 @@
         <v>12358940</v>
       </c>
       <c r="D20" s="1"/>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0.34728103571219704</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
@@ -6036,6 +6123,10 @@
         <v>27029734</v>
       </c>
       <c r="D21" s="1"/>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0.13854120756873103</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
@@ -6050,6 +6141,10 @@
         <v>8448801</v>
       </c>
       <c r="D22" s="1"/>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0.64417726006285003</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
@@ -6064,6 +6159,10 @@
         <v>1553665</v>
       </c>
       <c r="D23" s="1"/>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.64217084352439702</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
@@ -6078,6 +6177,10 @@
         <v>65956908</v>
       </c>
       <c r="D24" s="1"/>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0.24566921559716207</v>
+      </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
@@ -6092,6 +6195,10 @@
         <v>103046848</v>
       </c>
       <c r="D25" s="1"/>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0.24602210737060001</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
@@ -6106,6 +6213,10 @@
         <v>1234828</v>
       </c>
       <c r="D26" s="1"/>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0.35837227114176107</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
@@ -6120,6 +6231,10 @@
         <v>7600506</v>
       </c>
       <c r="D27" s="1"/>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0.34496420794893207</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
@@ -6134,6 +6249,10 @@
         <v>1090631</v>
       </c>
       <c r="D28" s="1"/>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0.68756430782958999</v>
+      </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
@@ -6148,6 +6267,10 @@
         <v>1418736</v>
       </c>
       <c r="D29" s="1"/>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0.76393229081237302</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
@@ -6162,6 +6285,10 @@
         <v>7541380</v>
       </c>
       <c r="D30" s="1"/>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0.27740282065227501</v>
+      </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
@@ -6176,6 +6303,10 @@
         <v>3795230</v>
       </c>
       <c r="D31" s="1"/>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0.578443052717729</v>
+      </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
@@ -6190,6 +6321,10 @@
         <v>9478973</v>
       </c>
       <c r="D32" s="1"/>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0.45380955762138603</v>
+      </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
@@ -6201,6 +6336,10 @@
         <v>9478973</v>
       </c>
       <c r="D33" s="1"/>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0.44200798501559707</v>
+      </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
@@ -6215,6 +6354,10 @@
         <v>3887740</v>
       </c>
       <c r="D34" s="1"/>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0.45290413322655299</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
@@ -6229,6 +6372,10 @@
         <v>2224812</v>
       </c>
       <c r="D35" s="1"/>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0.33332410592762007</v>
+      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
@@ -6243,6 +6390,10 @@
         <v>3245048</v>
       </c>
       <c r="D36" s="1"/>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>0.69514823309844098</v>
+      </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
@@ -6257,6 +6408,10 @@
         <v>3424774</v>
       </c>
       <c r="D37" s="1"/>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>0.46135336394388704</v>
+      </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
@@ -6271,6 +6426,10 @@
         <v>1818226</v>
       </c>
       <c r="D38" s="1"/>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>0.72648376607091392</v>
+      </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
@@ -6285,6 +6444,10 @@
         <v>844037</v>
       </c>
       <c r="D39" s="1"/>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>0.25576803162030398</v>
+      </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
@@ -6299,6 +6462,10 @@
         <v>448426</v>
       </c>
       <c r="D40" s="1"/>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>0.62390029995270102</v>
+      </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
@@ -6313,6 +6480,10 @@
         <v>3759821</v>
       </c>
       <c r="D41" s="1"/>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>0.31538248141172504</v>
+      </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
@@ -6327,6 +6498,10 @@
         <v>7364036</v>
       </c>
       <c r="D42" s="1"/>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>0.53435027316223405</v>
+      </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
@@ -6341,6 +6516,10 @@
         <v>648736</v>
       </c>
       <c r="D43" s="1"/>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>0.485700607276082</v>
+      </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
     </row>
@@ -6355,6 +6534,10 @@
         <v>4262100</v>
       </c>
       <c r="D44" s="1"/>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>0.27453747156222402</v>
+      </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
     </row>
@@ -6369,6 +6552,10 @@
         <v>12032796</v>
       </c>
       <c r="D45" s="1"/>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>0.26446905871473803</v>
+      </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
     </row>
@@ -6383,6 +6570,10 @@
         <v>4293102</v>
       </c>
       <c r="D46" s="1"/>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>0.24310394980413805</v>
+      </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
     </row>
@@ -6397,6 +6588,10 @@
         <v>1213151</v>
       </c>
       <c r="D47" s="1"/>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>0.68410157922210202</v>
+      </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
     </row>
@@ -6408,6 +6603,10 @@
         <v>1213151</v>
       </c>
       <c r="D48" s="1"/>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>0.66949123439652902</v>
+      </c>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
     </row>
@@ -6422,6 +6621,10 @@
         <v>1823588</v>
       </c>
       <c r="D49" s="1"/>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>0.34596925863376798</v>
+      </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
     </row>
@@ -6436,6 +6639,10 @@
         <v>1402985</v>
       </c>
       <c r="D50" s="1"/>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>0.64955151042731907</v>
+      </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
     </row>
@@ -6450,6 +6657,10 @@
         <v>3754728</v>
       </c>
       <c r="D51" s="1"/>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>0.37479999824795301</v>
+      </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
     </row>
@@ -6464,6 +6675,10 @@
         <v>5185403</v>
       </c>
       <c r="D52" s="1"/>
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>0.49484092116464401</v>
+      </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
     </row>
@@ -6478,6 +6693,10 @@
         <v>1665997</v>
       </c>
       <c r="D53" s="1"/>
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>0.72405033893597304</v>
+      </c>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
@@ -6492,6 +6711,10 @@
         <v>1944974</v>
       </c>
       <c r="D54" s="1"/>
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>0.26022350827032797</v>
+      </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
     </row>
@@ -6506,6 +6729,10 @@
         <v>1163023</v>
       </c>
       <c r="D55" s="1"/>
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>0.23991434312306106</v>
+      </c>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
@@ -6520,6 +6747,10 @@
         <v>31387096</v>
       </c>
       <c r="D56" s="1"/>
+      <c r="E56">
+        <f t="shared" si="0"/>
+        <v>0.27579316650414704</v>
+      </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
@@ -6534,6 +6765,10 @@
         <v>1053351</v>
       </c>
       <c r="D57" s="1"/>
+      <c r="E57">
+        <f t="shared" si="0"/>
+        <v>0.25661164400198505</v>
+      </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
     </row>
@@ -6548,6 +6783,10 @@
         <v>1007485</v>
       </c>
       <c r="D58" s="1"/>
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>0.390083461334295</v>
+      </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
     </row>
@@ -6562,6 +6801,10 @@
         <v>3201398</v>
       </c>
       <c r="D59" s="1"/>
+      <c r="E59">
+        <f t="shared" si="0"/>
+        <v>0.438920109085296</v>
+      </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
@@ -6576,6 +6819,10 @@
         <v>4141307</v>
       </c>
       <c r="D60" s="1"/>
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>0.52496612352932115</v>
+      </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
     </row>
@@ -6590,6 +6837,10 @@
         <v>2308894</v>
       </c>
       <c r="D61" s="1"/>
+      <c r="E61">
+        <f t="shared" si="0"/>
+        <v>0.71836930880010696</v>
+      </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
     </row>
@@ -6604,6 +6855,10 @@
         <v>1970490</v>
       </c>
       <c r="D62" s="1"/>
+      <c r="E62">
+        <f t="shared" si="0"/>
+        <v>0.31811109248701108</v>
+      </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
     </row>
@@ -6618,6 +6873,10 @@
         <v>5737909</v>
       </c>
       <c r="D63" s="1"/>
+      <c r="E63">
+        <f t="shared" si="0"/>
+        <v>0.23906355985253908</v>
+      </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
     </row>
@@ -6632,6 +6891,10 @@
         <v>16497745</v>
       </c>
       <c r="D64" s="1"/>
+      <c r="E64">
+        <f t="shared" si="0"/>
+        <v>0.27912214195962504</v>
+      </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
     </row>
@@ -6646,6 +6909,10 @@
         <v>7467403</v>
       </c>
       <c r="D65" s="1"/>
+      <c r="E65">
+        <f t="shared" si="0"/>
+        <v>0.25654077560220506</v>
+      </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
     </row>
@@ -6660,6 +6927,10 @@
         <v>12898326</v>
       </c>
       <c r="D66" s="1"/>
+      <c r="E66">
+        <f t="shared" si="0"/>
+        <v>0.30416595886310899</v>
+      </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
     </row>
@@ -6674,6 +6945,10 @@
         <v>2973444</v>
       </c>
       <c r="D67" s="1"/>
+      <c r="E67">
+        <f t="shared" ref="E67:E130" si="1">B67^(-1/6)</f>
+        <v>0.49680149144653807</v>
+      </c>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
     </row>
@@ -6688,6 +6963,10 @@
         <v>2601808</v>
       </c>
       <c r="D68" s="1"/>
+      <c r="E68">
+        <f t="shared" si="1"/>
+        <v>0.214637190367996</v>
+      </c>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
     </row>
@@ -6702,6 +6981,10 @@
         <v>3453665</v>
       </c>
       <c r="D69" s="1"/>
+      <c r="E69">
+        <f t="shared" si="1"/>
+        <v>0.42883578191428101</v>
+      </c>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
     </row>
@@ -6716,6 +6999,10 @@
         <v>1661018</v>
       </c>
       <c r="D70" s="1"/>
+      <c r="E70">
+        <f t="shared" si="1"/>
+        <v>0.44483286310205794</v>
+      </c>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
     </row>
@@ -6730,6 +7017,10 @@
         <v>2384839</v>
       </c>
       <c r="D71" s="1"/>
+      <c r="E71">
+        <f t="shared" si="1"/>
+        <v>0.485947906737137</v>
+      </c>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
     </row>
@@ -6744,6 +7035,10 @@
         <v>4557164</v>
       </c>
       <c r="D72" s="1"/>
+      <c r="E72">
+        <f t="shared" si="1"/>
+        <v>0.24052390379006794</v>
+      </c>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
     </row>
@@ -6758,6 +7053,10 @@
         <v>12711756</v>
       </c>
       <c r="D73" s="1"/>
+      <c r="E73">
+        <f t="shared" si="1"/>
+        <v>0.27610200675411206</v>
+      </c>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
     </row>
@@ -6772,6 +7071,10 @@
         <v>9870797</v>
       </c>
       <c r="D74" s="1"/>
+      <c r="E74">
+        <f t="shared" si="1"/>
+        <v>0.92394501529716899</v>
+      </c>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
     </row>
@@ -6786,6 +7089,10 @@
         <v>3637665</v>
       </c>
       <c r="D75" s="1"/>
+      <c r="E75">
+        <f t="shared" si="1"/>
+        <v>0.238941415002413</v>
+      </c>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
     </row>
@@ -6800,6 +7107,10 @@
         <v>11901120</v>
       </c>
       <c r="D76" s="1"/>
+      <c r="E76">
+        <f t="shared" si="1"/>
+        <v>0.27705257892261703</v>
+      </c>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
     </row>
@@ -6814,6 +7125,10 @@
         <v>6909822</v>
       </c>
       <c r="D77" s="1"/>
+      <c r="E77">
+        <f t="shared" si="1"/>
+        <v>0.21302148789037803</v>
+      </c>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
     </row>
@@ -6828,6 +7143,10 @@
         <v>3425331</v>
       </c>
       <c r="D78" s="1"/>
+      <c r="E78">
+        <f t="shared" si="1"/>
+        <v>0.54605615115113304</v>
+      </c>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
     </row>
@@ -6842,6 +7161,10 @@
         <v>9127447</v>
       </c>
       <c r="D79" s="1"/>
+      <c r="E79">
+        <f t="shared" si="1"/>
+        <v>0.42313304666907797</v>
+      </c>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
     </row>
@@ -6856,6 +7179,10 @@
         <v>6527978</v>
       </c>
       <c r="D80" s="1"/>
+      <c r="E80">
+        <f t="shared" si="1"/>
+        <v>0.53467214423111598</v>
+      </c>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
     </row>
@@ -6870,6 +7197,10 @@
         <v>2420787</v>
       </c>
       <c r="D81" s="1"/>
+      <c r="E81">
+        <f t="shared" si="1"/>
+        <v>0.63211279874135895</v>
+      </c>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
     </row>
@@ -6884,6 +7215,10 @@
         <v>2509800</v>
       </c>
       <c r="D82" s="1"/>
+      <c r="E82">
+        <f t="shared" si="1"/>
+        <v>0.42894190853654107</v>
+      </c>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
     </row>
@@ -6898,6 +7233,10 @@
         <v>3473186</v>
       </c>
       <c r="D83" s="1"/>
+      <c r="E83">
+        <f t="shared" si="1"/>
+        <v>0.23852552410416997</v>
+      </c>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
     </row>
@@ -6912,6 +7251,10 @@
         <v>2345788</v>
       </c>
       <c r="D84" s="1"/>
+      <c r="E84">
+        <f t="shared" si="1"/>
+        <v>0.27459734776513001</v>
+      </c>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
     </row>
@@ -6926,6 +7269,10 @@
         <v>2514887</v>
       </c>
       <c r="D85" s="1"/>
+      <c r="E85">
+        <f t="shared" si="1"/>
+        <v>0.25787901756611403</v>
+      </c>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
     </row>
@@ -6940,6 +7287,10 @@
         <v>4753880</v>
       </c>
       <c r="D86" s="1"/>
+      <c r="E86">
+        <f t="shared" si="1"/>
+        <v>0.223549530314399</v>
+      </c>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
     </row>
@@ -6954,6 +7305,10 @@
         <v>2539644</v>
       </c>
       <c r="D87" s="1"/>
+      <c r="E87">
+        <f t="shared" si="1"/>
+        <v>0.424151270013992</v>
+      </c>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
     </row>
@@ -6968,6 +7323,10 @@
         <v>3996778</v>
       </c>
       <c r="D88" s="1"/>
+      <c r="E88">
+        <f t="shared" si="1"/>
+        <v>0.35611531062345503</v>
+      </c>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
     </row>
@@ -6982,6 +7341,10 @@
         <v>2332954</v>
       </c>
       <c r="D89" s="1"/>
+      <c r="E89">
+        <f t="shared" si="1"/>
+        <v>0.46013176457604399</v>
+      </c>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
     </row>
@@ -6996,6 +7359,10 @@
         <v>21634050</v>
       </c>
       <c r="D90" s="1"/>
+      <c r="E90">
+        <f t="shared" si="1"/>
+        <v>0.139143407037984</v>
+      </c>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
     </row>
@@ -7010,6 +7377,10 @@
         <v>4623962</v>
       </c>
       <c r="D91" s="1"/>
+      <c r="E91">
+        <f t="shared" si="1"/>
+        <v>0.63966715298677801</v>
+      </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
     </row>
@@ -7024,6 +7395,10 @@
         <v>36924364</v>
       </c>
       <c r="D92" s="1"/>
+      <c r="E92">
+        <f t="shared" si="1"/>
+        <v>0.260230900134509</v>
+      </c>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
     </row>
@@ -7038,6 +7413,10 @@
         <v>25188170</v>
       </c>
       <c r="D93" s="1"/>
+      <c r="E93">
+        <f t="shared" si="1"/>
+        <v>0.50989222529330602</v>
+      </c>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
     </row>
@@ -7052,6 +7431,10 @@
         <v>1408504</v>
       </c>
       <c r="D94" s="1"/>
+      <c r="E94">
+        <f t="shared" si="1"/>
+        <v>0.722951236296283</v>
+      </c>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
     </row>
@@ -7066,6 +7449,10 @@
         <v>4755548</v>
       </c>
       <c r="D95" s="1"/>
+      <c r="E95">
+        <f t="shared" si="1"/>
+        <v>0.46895647226389697</v>
+      </c>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
     </row>
@@ -7080,6 +7467,10 @@
         <v>3874683</v>
       </c>
       <c r="D96" s="1"/>
+      <c r="E96">
+        <f t="shared" si="1"/>
+        <v>0.57950001707001697</v>
+      </c>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
     </row>
@@ -7094,6 +7485,10 @@
         <v>2929694</v>
       </c>
       <c r="D97" s="1"/>
+      <c r="E97">
+        <f t="shared" si="1"/>
+        <v>0.28240665710752305</v>
+      </c>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
     </row>
@@ -7108,6 +7503,10 @@
         <v>3026562</v>
       </c>
       <c r="D98" s="1"/>
+      <c r="E98">
+        <f t="shared" si="1"/>
+        <v>0.237893565275128</v>
+      </c>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
     </row>
@@ -7122,6 +7521,10 @@
         <v>23331556</v>
       </c>
       <c r="D99" s="1"/>
+      <c r="E99">
+        <f t="shared" si="1"/>
+        <v>0.27199041879430302</v>
+      </c>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
@@ -7136,6 +7539,10 @@
         <v>1333352</v>
       </c>
       <c r="D100" s="1"/>
+      <c r="E100">
+        <f t="shared" si="1"/>
+        <v>0.25580155788858905</v>
+      </c>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
     </row>
@@ -7150,6 +7557,10 @@
         <v>4641299</v>
       </c>
       <c r="D101" s="1"/>
+      <c r="E101">
+        <f t="shared" si="1"/>
+        <v>0.58166545439436501</v>
+      </c>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
     </row>
@@ -7164,6 +7575,10 @@
         <v>2650738</v>
       </c>
       <c r="D102" s="1"/>
+      <c r="E102">
+        <f t="shared" si="1"/>
+        <v>0.389442979482503</v>
+      </c>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
     </row>
@@ -7178,6 +7593,10 @@
         <v>2723156</v>
       </c>
       <c r="D103" s="1"/>
+      <c r="E103">
+        <f t="shared" si="1"/>
+        <v>0.66261261315974396</v>
+      </c>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
     </row>
@@ -7192,6 +7611,10 @@
         <v>1554034</v>
       </c>
       <c r="D104" s="1"/>
+      <c r="E104">
+        <f t="shared" si="1"/>
+        <v>0.21435669032812202</v>
+      </c>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
     </row>
@@ -7206,6 +7629,10 @@
         <v>5050146</v>
       </c>
       <c r="D105" s="1"/>
+      <c r="E105">
+        <f t="shared" si="1"/>
+        <v>0.66261261315974396</v>
+      </c>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
     </row>
@@ -7220,6 +7647,10 @@
         <v>7179130</v>
       </c>
       <c r="D106" s="1"/>
+      <c r="E106">
+        <f t="shared" si="1"/>
+        <v>0.21435669032812202</v>
+      </c>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
     </row>
@@ -7234,6 +7665,10 @@
         <v>1525712</v>
       </c>
       <c r="D107" s="1"/>
+      <c r="E107">
+        <f t="shared" si="1"/>
+        <v>0.380707594117971</v>
+      </c>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
     </row>
@@ -7248,6 +7683,10 @@
         <v>1980709</v>
       </c>
       <c r="D108" s="1"/>
+      <c r="E108">
+        <f t="shared" si="1"/>
+        <v>0.407075943833486</v>
+      </c>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
     </row>
@@ -7262,6 +7701,10 @@
         <v>3289502</v>
       </c>
       <c r="D109" s="1"/>
+      <c r="E109">
+        <f t="shared" si="1"/>
+        <v>0.4718320644427641</v>
+      </c>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
     </row>
@@ -7276,6 +7719,10 @@
         <v>5455976</v>
       </c>
       <c r="D110" s="1"/>
+      <c r="E110">
+        <f t="shared" si="1"/>
+        <v>0.27977717143968406</v>
+      </c>
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
     </row>
@@ -7290,6 +7737,10 @@
         <v>10928946</v>
       </c>
       <c r="D111" s="1"/>
+      <c r="E111">
+        <f t="shared" si="1"/>
+        <v>0.23991688986255696</v>
+      </c>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
     </row>
@@ -7304,6 +7755,10 @@
         <v>60550944</v>
       </c>
       <c r="D112" s="1"/>
+      <c r="E112">
+        <f t="shared" si="1"/>
+        <v>0.27826413670072103</v>
+      </c>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
     </row>
@@ -7318,6 +7773,10 @@
         <v>2418320</v>
       </c>
       <c r="D113" s="1"/>
+      <c r="E113">
+        <f t="shared" si="1"/>
+        <v>0.38946867153509601</v>
+      </c>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
     </row>
@@ -7332,6 +7791,10 @@
         <v>1271135</v>
       </c>
       <c r="D114" s="1"/>
+      <c r="E114">
+        <f t="shared" si="1"/>
+        <v>0.17774514834833</v>
+      </c>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
     </row>
@@ -7346,6 +7809,10 @@
         <v>1357090</v>
       </c>
       <c r="D115" s="1"/>
+      <c r="E115">
+        <f t="shared" si="1"/>
+        <v>0.25096836689856505</v>
+      </c>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
     </row>
@@ -7360,6 +7827,10 @@
         <v>2331125</v>
       </c>
       <c r="D116" s="1"/>
+      <c r="E116">
+        <f t="shared" si="1"/>
+        <v>0.29043555132273108</v>
+      </c>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
     </row>
@@ -7374,6 +7845,10 @@
         <v>1630330</v>
       </c>
       <c r="D117" s="1"/>
+      <c r="E117">
+        <f t="shared" si="1"/>
+        <v>0.49619751726399508</v>
+      </c>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
@@ -7388,6 +7863,10 @@
         <v>6138712</v>
       </c>
       <c r="D118" s="1"/>
+      <c r="E118">
+        <f t="shared" si="1"/>
+        <v>0.44097724884418305</v>
+      </c>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
     </row>
@@ -7402,6 +7881,10 @@
         <v>1455771</v>
       </c>
       <c r="D119" s="1"/>
+      <c r="E119">
+        <f t="shared" si="1"/>
+        <v>0.45141613388153795</v>
+      </c>
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
     </row>
@@ -7416,6 +7899,10 @@
         <v>1504642</v>
       </c>
       <c r="D120" s="1"/>
+      <c r="E120">
+        <f t="shared" si="1"/>
+        <v>0.505027651306721</v>
+      </c>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
     </row>
@@ -7430,6 +7917,10 @@
         <v>7398854</v>
       </c>
       <c r="D121" s="1"/>
+      <c r="E121">
+        <f t="shared" si="1"/>
+        <v>0.64737093142902802</v>
+      </c>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
     </row>
@@ -7441,6 +7932,10 @@
         <v>7398854</v>
       </c>
       <c r="D122" s="1"/>
+      <c r="E122">
+        <f t="shared" si="1"/>
+        <v>0.77741419774842802</v>
+      </c>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
     </row>
@@ -7455,6 +7950,10 @@
         <v>1111251</v>
       </c>
       <c r="D123" s="1"/>
+      <c r="E123">
+        <f t="shared" si="1"/>
+        <v>0.23816311343203203</v>
+      </c>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
     </row>
@@ -7469,6 +7968,10 @@
         <v>31141268</v>
       </c>
       <c r="D124" s="1"/>
+      <c r="E124">
+        <f t="shared" si="1"/>
+        <v>0.272106705845444</v>
+      </c>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
     </row>
@@ -7483,6 +7986,10 @@
         <v>2229518</v>
       </c>
       <c r="D125" s="1"/>
+      <c r="E125">
+        <f t="shared" si="1"/>
+        <v>0.25194480914610207</v>
+      </c>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
     </row>
@@ -7497,6 +8004,10 @@
         <v>9303714</v>
       </c>
       <c r="D126" s="1"/>
+      <c r="E126">
+        <f t="shared" si="1"/>
+        <v>0.603572727012889</v>
+      </c>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
     </row>
@@ -7511,6 +8022,10 @@
         <v>627384</v>
       </c>
       <c r="D127" s="1"/>
+      <c r="E127">
+        <f t="shared" si="1"/>
+        <v>0.27464974076932103</v>
+      </c>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
     </row>
@@ -7525,6 +8040,10 @@
         <v>3489148</v>
       </c>
       <c r="D128" s="1"/>
+      <c r="E128">
+        <f t="shared" si="1"/>
+        <v>0.36010131286238906</v>
+      </c>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
     </row>
@@ -7539,6 +8058,10 @@
         <v>958734</v>
       </c>
       <c r="D129" s="1"/>
+      <c r="E129">
+        <f t="shared" si="1"/>
+        <v>0.27422765105469005</v>
+      </c>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
     </row>
@@ -7553,6 +8076,10 @@
         <v>2998805</v>
       </c>
       <c r="D130" s="1"/>
+      <c r="E130">
+        <f t="shared" si="1"/>
+        <v>0.64553111576227995</v>
+      </c>
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
     </row>
@@ -7567,6 +8094,10 @@
         <v>1575453</v>
       </c>
       <c r="D131" s="1"/>
+      <c r="E131">
+        <f t="shared" ref="E131:E194" si="2">B131^(-1/6)</f>
+        <v>0.344809858358265</v>
+      </c>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
     </row>
@@ -7581,6 +8112,10 @@
         <v>764261</v>
       </c>
       <c r="D132" s="1"/>
+      <c r="E132">
+        <f t="shared" si="2"/>
+        <v>0.30116343278029406</v>
+      </c>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
     </row>
@@ -7592,6 +8127,10 @@
         <v>764261</v>
       </c>
       <c r="D133" s="1"/>
+      <c r="E133">
+        <f t="shared" si="2"/>
+        <v>0.21319220858791602</v>
+      </c>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
     </row>
@@ -7603,6 +8142,10 @@
         <v>764261</v>
       </c>
       <c r="D134" s="1"/>
+      <c r="E134">
+        <f t="shared" si="2"/>
+        <v>0.10889331990325801</v>
+      </c>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
     </row>
@@ -7617,6 +8160,10 @@
         <v>4624204</v>
       </c>
       <c r="D135" s="1"/>
+      <c r="E135">
+        <f t="shared" si="2"/>
+        <v>0.63766354638846412</v>
+      </c>
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
     </row>
@@ -7628,6 +8175,10 @@
         <v>4624204</v>
       </c>
       <c r="D136" s="1"/>
+      <c r="E136">
+        <f t="shared" si="2"/>
+        <v>0.528764309247854</v>
+      </c>
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
     </row>
@@ -7639,6 +8190,10 @@
         <v>4624204</v>
       </c>
       <c r="D137" s="1"/>
+      <c r="E137">
+        <f t="shared" si="2"/>
+        <v>0.38684633277530506</v>
+      </c>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
     </row>
@@ -7653,6 +8208,10 @@
         <v>1789150</v>
       </c>
       <c r="D138" s="1"/>
+      <c r="E138">
+        <f t="shared" si="2"/>
+        <v>0.35867449740478602</v>
+      </c>
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
     </row>
@@ -7667,6 +8226,10 @@
         <v>2535420</v>
       </c>
       <c r="D139" s="1"/>
+      <c r="E139">
+        <f t="shared" si="2"/>
+        <v>0.47505185165292502</v>
+      </c>
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
     </row>
@@ -7681,6 +8244,10 @@
         <v>1450116</v>
       </c>
       <c r="D140" s="1"/>
+      <c r="E140">
+        <f t="shared" si="2"/>
+        <v>0.68497401586710205</v>
+      </c>
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
     </row>
@@ -7695,6 +8262,10 @@
         <v>1260504</v>
       </c>
       <c r="D141" s="1"/>
+      <c r="E141">
+        <f t="shared" si="2"/>
+        <v>0.719819787316478</v>
+      </c>
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
     </row>
@@ -7709,6 +8280,10 @@
         <v>3135101</v>
       </c>
       <c r="D142" s="1"/>
+      <c r="E142">
+        <f t="shared" si="2"/>
+        <v>0.23993958430446002</v>
+      </c>
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
     </row>
@@ -7723,6 +8298,10 @@
         <v>786986</v>
       </c>
       <c r="D143" s="1"/>
+      <c r="E143">
+        <f t="shared" si="2"/>
+        <v>0.28154504194330499</v>
+      </c>
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
     </row>
@@ -7737,6 +8316,10 @@
         <v>5538548</v>
       </c>
       <c r="D144" s="1"/>
+      <c r="E144">
+        <f t="shared" si="2"/>
+        <v>0.30652189126118107</v>
+      </c>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
     </row>
@@ -7751,6 +8334,10 @@
         <v>10205974</v>
       </c>
       <c r="D145" s="1"/>
+      <c r="E145">
+        <f t="shared" si="2"/>
+        <v>0.25581520805854907</v>
+      </c>
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
     </row>
@@ -7765,6 +8352,10 @@
         <v>2956913</v>
       </c>
       <c r="D146" s="1"/>
+      <c r="E146">
+        <f t="shared" si="2"/>
+        <v>0.37950954124757502</v>
+      </c>
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
     </row>
@@ -7779,6 +8370,10 @@
         <v>10840755</v>
       </c>
       <c r="D147" s="1"/>
+      <c r="E147">
+        <f t="shared" si="2"/>
+        <v>0.38965874744609502</v>
+      </c>
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
     </row>
@@ -7793,6 +8388,10 @@
         <v>3494985</v>
       </c>
       <c r="D148" s="1"/>
+      <c r="E148">
+        <f t="shared" si="2"/>
+        <v>0.27349594453425008</v>
+      </c>
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
     </row>
@@ -7807,6 +8406,10 @@
         <v>4774056</v>
       </c>
       <c r="D149" s="1"/>
+      <c r="E149">
+        <f t="shared" si="2"/>
+        <v>0.41424921404710197</v>
+      </c>
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
     </row>
@@ -7821,6 +8424,10 @@
         <v>5431832</v>
       </c>
       <c r="D150" s="1"/>
+      <c r="E150">
+        <f t="shared" si="2"/>
+        <v>0.30090209815155106</v>
+      </c>
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
     </row>
@@ -7835,6 +8442,10 @@
         <v>4834980</v>
       </c>
       <c r="D151" s="1"/>
+      <c r="E151">
+        <f t="shared" si="2"/>
+        <v>0.63848948654595805</v>
+      </c>
       <c r="G151" s="1"/>
       <c r="H151" s="1"/>
     </row>
@@ -7849,6 +8460,10 @@
         <v>4786616</v>
       </c>
       <c r="D152" s="1"/>
+      <c r="E152">
+        <f t="shared" si="2"/>
+        <v>0.69483834307639403</v>
+      </c>
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
     </row>
@@ -7863,6 +8478,10 @@
         <v>2529986</v>
       </c>
       <c r="D153" s="1"/>
+      <c r="E153">
+        <f t="shared" si="2"/>
+        <v>0.44997343487489005</v>
+      </c>
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
     </row>
@@ -7877,6 +8496,10 @@
         <v>2772034</v>
       </c>
       <c r="D154" s="1"/>
+      <c r="E154">
+        <f t="shared" si="2"/>
+        <v>0.627375895406588</v>
+      </c>
       <c r="G154" s="1"/>
       <c r="H154" s="1"/>
     </row>
@@ -7891,6 +8514,10 @@
         <v>3186041</v>
       </c>
       <c r="D155" s="1"/>
+      <c r="E155">
+        <f t="shared" si="2"/>
+        <v>0.55382471933837107</v>
+      </c>
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
     </row>
@@ -7905,6 +8532,10 @@
         <v>2982985</v>
       </c>
       <c r="D156" s="1"/>
+      <c r="E156">
+        <f t="shared" si="2"/>
+        <v>0.66811448799231699</v>
+      </c>
       <c r="G156" s="1"/>
       <c r="H156" s="1"/>
     </row>
@@ -7919,6 +8550,10 @@
         <v>723682</v>
       </c>
       <c r="D157" s="1"/>
+      <c r="E157">
+        <f t="shared" si="2"/>
+        <v>0.17797891857453199</v>
+      </c>
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
     </row>
@@ -7933,6 +8568,10 @@
         <v>2542702</v>
       </c>
       <c r="D158" s="1"/>
+      <c r="E158">
+        <f t="shared" si="2"/>
+        <v>0.64817196161688095</v>
+      </c>
       <c r="G158" s="1"/>
       <c r="H158" s="1"/>
     </row>
@@ -7947,6 +8586,10 @@
         <v>2678700</v>
       </c>
       <c r="D159" s="1"/>
+      <c r="E159">
+        <f t="shared" si="2"/>
+        <v>0.33791929231373102</v>
+      </c>
       <c r="G159" s="1"/>
       <c r="H159" s="1"/>
     </row>
@@ -7961,6 +8604,10 @@
         <v>4920920</v>
       </c>
       <c r="D160" s="1"/>
+      <c r="E160">
+        <f t="shared" si="2"/>
+        <v>0.28899466903912707</v>
+      </c>
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
     </row>
@@ -7972,6 +8619,10 @@
         <v>4920920</v>
       </c>
       <c r="D161" s="1"/>
+      <c r="E161">
+        <f t="shared" si="2"/>
+        <v>0.32453596486367908</v>
+      </c>
       <c r="G161" s="1"/>
       <c r="H161" s="1"/>
     </row>
@@ -7983,6 +8634,10 @@
         <v>4920920</v>
       </c>
       <c r="D162" s="1"/>
+      <c r="E162">
+        <f t="shared" si="2"/>
+        <v>0.25868326346890702</v>
+      </c>
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
     </row>
@@ -7997,6 +8652,10 @@
         <v>6172494</v>
       </c>
       <c r="D163" s="1"/>
+      <c r="E163">
+        <f t="shared" si="2"/>
+        <v>0.28235733385544104</v>
+      </c>
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
     </row>
@@ -8008,6 +8667,10 @@
         <v>6172494</v>
       </c>
       <c r="D164" s="1"/>
+      <c r="E164">
+        <f t="shared" si="2"/>
+        <v>0.40444150394189399</v>
+      </c>
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
     </row>
@@ -8019,6 +8682,10 @@
         <v>6172494</v>
       </c>
       <c r="D165" s="1"/>
+      <c r="E165">
+        <f t="shared" si="2"/>
+        <v>0.49262836468460702</v>
+      </c>
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
     </row>
@@ -8033,6 +8700,10 @@
         <v>10077953</v>
       </c>
       <c r="D166" s="1"/>
+      <c r="E166">
+        <f t="shared" si="2"/>
+        <v>0.27394172757100299</v>
+      </c>
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
     </row>
@@ -8047,6 +8718,10 @@
         <v>1260391</v>
       </c>
       <c r="D167" s="1"/>
+      <c r="E167">
+        <f t="shared" si="2"/>
+        <v>0.41213804652786307</v>
+      </c>
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
     </row>
@@ -8061,6 +8736,10 @@
         <v>1971224</v>
       </c>
       <c r="D168" s="1"/>
+      <c r="E168">
+        <f t="shared" si="2"/>
+        <v>0.51599836582779801</v>
+      </c>
       <c r="G168" s="1"/>
       <c r="H168" s="1"/>
     </row>
@@ -8072,6 +8751,10 @@
         <v>1971224</v>
       </c>
       <c r="D169" s="1"/>
+      <c r="E169">
+        <f t="shared" si="2"/>
+        <v>0.38648438651323602</v>
+      </c>
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
     </row>
@@ -8083,6 +8766,10 @@
         <v>1971224</v>
       </c>
       <c r="D170" s="1"/>
+      <c r="E170">
+        <f t="shared" si="2"/>
+        <v>0.46464052634681002</v>
+      </c>
       <c r="G170" s="1"/>
       <c r="H170" s="1"/>
     </row>
@@ -8097,6 +8784,10 @@
         <v>9960204</v>
       </c>
       <c r="D171" s="1"/>
+      <c r="E171">
+        <f t="shared" si="2"/>
+        <v>0.108955086000567</v>
+      </c>
       <c r="G171" s="1"/>
       <c r="H171" s="1"/>
     </row>
@@ -8108,6 +8799,10 @@
         <v>9960204</v>
       </c>
       <c r="D172" s="1"/>
+      <c r="E172">
+        <f t="shared" si="2"/>
+        <v>0.108950220337362</v>
+      </c>
       <c r="G172" s="1"/>
       <c r="H172" s="1"/>
     </row>
@@ -8119,6 +8814,10 @@
         <v>9960204</v>
       </c>
       <c r="D173" s="1"/>
+      <c r="E173">
+        <f t="shared" si="2"/>
+        <v>0.27256011827059201</v>
+      </c>
       <c r="G173" s="1"/>
       <c r="H173" s="1"/>
     </row>
@@ -8133,6 +8832,10 @@
         <v>1529686</v>
       </c>
       <c r="D174" s="1"/>
+      <c r="E174">
+        <f t="shared" si="2"/>
+        <v>0.326251447044765</v>
+      </c>
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
     </row>
@@ -8144,6 +8847,10 @@
         <v>1529686</v>
       </c>
       <c r="D175" s="1"/>
+      <c r="E175">
+        <f t="shared" si="2"/>
+        <v>0.42545700022888511</v>
+      </c>
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
     </row>
@@ -8155,6 +8862,10 @@
         <v>1529686</v>
       </c>
       <c r="D176" s="1"/>
+      <c r="E176">
+        <f t="shared" si="2"/>
+        <v>0.65479689789163698</v>
+      </c>
       <c r="G176" s="1"/>
       <c r="H176" s="1"/>
     </row>
@@ -8169,6 +8880,10 @@
         <v>1689700</v>
       </c>
       <c r="D177" s="1"/>
+      <c r="E177">
+        <f t="shared" si="2"/>
+        <v>0.833141687135452</v>
+      </c>
       <c r="G177" s="1"/>
       <c r="H177" s="1"/>
     </row>
@@ -8183,6 +8898,10 @@
         <v>3556184</v>
       </c>
       <c r="D178" s="1"/>
+      <c r="E178">
+        <f t="shared" si="2"/>
+        <v>0.61634778880422303</v>
+      </c>
       <c r="G178" s="1"/>
       <c r="H178" s="1"/>
     </row>
@@ -8197,6 +8916,10 @@
         <v>2296770</v>
       </c>
       <c r="D179" s="1"/>
+      <c r="E179">
+        <f t="shared" si="2"/>
+        <v>0.37921062185336107</v>
+      </c>
       <c r="G179" s="1"/>
       <c r="H179" s="1"/>
     </row>
@@ -8211,6 +8934,10 @@
         <v>3186601</v>
       </c>
       <c r="D180" s="1"/>
+      <c r="E180">
+        <f t="shared" si="2"/>
+        <v>0.24070243462020999</v>
+      </c>
       <c r="G180" s="1"/>
       <c r="H180" s="1"/>
     </row>
@@ -8225,6 +8952,10 @@
         <v>16820308</v>
       </c>
       <c r="D181" s="1"/>
+      <c r="E181">
+        <f t="shared" si="2"/>
+        <v>0.28158202745439598</v>
+      </c>
       <c r="G181" s="1"/>
       <c r="H181" s="1"/>
     </row>
@@ -8239,6 +8970,10 @@
         <v>8265592</v>
       </c>
       <c r="D182" s="1"/>
+      <c r="E182">
+        <f t="shared" si="2"/>
+        <v>0.22860196156702803</v>
+      </c>
       <c r="G182" s="1"/>
       <c r="H182" s="1"/>
     </row>
@@ -8253,6 +8988,10 @@
         <v>5714582</v>
       </c>
       <c r="D183" s="1"/>
+      <c r="E183">
+        <f t="shared" si="2"/>
+        <v>0.25336396684722901</v>
+      </c>
       <c r="G183" s="1"/>
       <c r="H183" s="1"/>
     </row>
@@ -8267,6 +9006,10 @@
         <v>1429138</v>
       </c>
       <c r="D184" s="1"/>
+      <c r="E184">
+        <f t="shared" si="2"/>
+        <v>0.80054748396731212</v>
+      </c>
       <c r="G184" s="1"/>
       <c r="H184" s="1"/>
     </row>
@@ -8281,6 +9024,10 @@
         <v>3785839</v>
       </c>
       <c r="D185" s="1"/>
+      <c r="E185">
+        <f t="shared" si="2"/>
+        <v>0.81038624140142912</v>
+      </c>
       <c r="G185" s="1"/>
       <c r="H185" s="1"/>
     </row>
@@ -8295,6 +9042,10 @@
         <v>2631506</v>
       </c>
       <c r="D186" s="1"/>
+      <c r="E186">
+        <f t="shared" si="2"/>
+        <v>0.22343157204754902</v>
+      </c>
       <c r="G186" s="1"/>
       <c r="H186" s="1"/>
     </row>
@@ -8309,6 +9060,10 @@
         <v>3832483</v>
       </c>
       <c r="D187" s="1"/>
+      <c r="E187">
+        <f t="shared" si="2"/>
+        <v>0.35268578234915404</v>
+      </c>
       <c r="G187" s="1"/>
       <c r="H187" s="1"/>
     </row>
@@ -8323,6 +9078,10 @@
         <v>16042746</v>
       </c>
       <c r="D188" s="1"/>
+      <c r="E188">
+        <f t="shared" si="2"/>
+        <v>0.13951000526622406</v>
+      </c>
       <c r="G188" s="1"/>
       <c r="H188" s="1"/>
     </row>
@@ -8337,6 +9096,10 @@
         <v>6889770</v>
       </c>
       <c r="D189" s="1"/>
+      <c r="E189">
+        <f t="shared" si="2"/>
+        <v>0.75954663468999895</v>
+      </c>
       <c r="G189" s="1"/>
       <c r="H189" s="1"/>
     </row>
@@ -8351,6 +9114,10 @@
         <v>831713</v>
       </c>
       <c r="D190" s="1"/>
+      <c r="E190">
+        <f t="shared" si="2"/>
+        <v>0.50845074695333503</v>
+      </c>
       <c r="G190" s="1"/>
       <c r="H190" s="1"/>
     </row>
@@ -8365,6 +9132,10 @@
         <v>10140926</v>
       </c>
       <c r="D191" s="1"/>
+      <c r="E191">
+        <f t="shared" si="2"/>
+        <v>0.360583543805365</v>
+      </c>
       <c r="G191" s="1"/>
       <c r="H191" s="1"/>
     </row>
@@ -8379,6 +9150,10 @@
         <v>1573897</v>
       </c>
       <c r="D192" s="1"/>
+      <c r="E192">
+        <f t="shared" si="2"/>
+        <v>0.62727886571737701</v>
+      </c>
       <c r="G192" s="1"/>
       <c r="H192" s="1"/>
     </row>
@@ -8393,6 +9168,10 @@
         <v>2813260</v>
       </c>
       <c r="D193" s="1"/>
+      <c r="E193">
+        <f t="shared" si="2"/>
+        <v>0.33881676084777101</v>
+      </c>
       <c r="G193" s="1"/>
       <c r="H193" s="1"/>
     </row>
@@ -8404,6 +9183,10 @@
         <v>2813260</v>
       </c>
       <c r="D194" s="1"/>
+      <c r="E194">
+        <f t="shared" si="2"/>
+        <v>0.40590566170888798</v>
+      </c>
       <c r="G194" s="1"/>
       <c r="H194" s="1"/>
     </row>
@@ -8418,6 +9201,10 @@
         <v>4583458</v>
       </c>
       <c r="D195" s="1"/>
+      <c r="E195">
+        <f t="shared" ref="E195:E207" si="3">B195^(-1/6)</f>
+        <v>0.240531711848747</v>
+      </c>
       <c r="G195" s="1"/>
       <c r="H195" s="1"/>
     </row>
@@ -8432,6 +9219,10 @@
         <v>19898080</v>
       </c>
       <c r="D196" s="1"/>
+      <c r="E196">
+        <f t="shared" si="3"/>
+        <v>0.37986082035579</v>
+      </c>
       <c r="G196" s="1"/>
       <c r="H196" s="1"/>
     </row>
@@ -8443,6 +9234,10 @@
         <v>19898080</v>
       </c>
       <c r="D197" s="1"/>
+      <c r="E197">
+        <f t="shared" si="3"/>
+        <v>0.27116185629276102</v>
+      </c>
       <c r="G197" s="1"/>
       <c r="H197" s="1"/>
     </row>
@@ -8457,6 +9252,10 @@
         <v>1707462</v>
       </c>
       <c r="D198" s="1"/>
+      <c r="E198">
+        <f t="shared" si="3"/>
+        <v>0.15305958615604204</v>
+      </c>
       <c r="G198" s="1"/>
       <c r="H198" s="1"/>
     </row>
@@ -8471,6 +9270,10 @@
         <v>13501586</v>
       </c>
       <c r="D199" s="1"/>
+      <c r="E199">
+        <f t="shared" si="3"/>
+        <v>0.24123682037488903</v>
+      </c>
       <c r="G199" s="1"/>
       <c r="H199" s="1"/>
     </row>
@@ -8482,6 +9285,10 @@
         <v>13501586</v>
       </c>
       <c r="D200" s="1"/>
+      <c r="E200">
+        <f t="shared" si="3"/>
+        <v>0.21393467634043301</v>
+      </c>
       <c r="G200" s="1"/>
       <c r="H200" s="1"/>
     </row>
@@ -8496,6 +9303,10 @@
         <v>1849326</v>
       </c>
       <c r="D201" s="1"/>
+      <c r="E201">
+        <f t="shared" si="3"/>
+        <v>0.25511017485849208</v>
+      </c>
       <c r="G201" s="1"/>
       <c r="H201" s="1"/>
     </row>
@@ -8510,6 +9321,10 @@
         <v>5570253</v>
       </c>
       <c r="D202" s="1"/>
+      <c r="E202">
+        <f t="shared" si="3"/>
+        <v>0.46211102831540307</v>
+      </c>
       <c r="G202" s="1"/>
       <c r="H202" s="1"/>
     </row>
@@ -8521,6 +9336,10 @@
         <v>5570253</v>
       </c>
       <c r="D203" s="1"/>
+      <c r="E203">
+        <f t="shared" si="3"/>
+        <v>0.34005662745347298</v>
+      </c>
       <c r="G203" s="1"/>
       <c r="H203" s="1"/>
     </row>
@@ -8535,6 +9354,10 @@
         <v>54772184</v>
       </c>
       <c r="D204" s="1"/>
+      <c r="E204">
+        <f t="shared" si="3"/>
+        <v>0.13877581014113702</v>
+      </c>
       <c r="G204" s="1"/>
       <c r="H204" s="1"/>
     </row>
@@ -8546,6 +9369,10 @@
         <v>54772184</v>
       </c>
       <c r="D205" s="1"/>
+      <c r="E205">
+        <f t="shared" si="3"/>
+        <v>0.33768379460371906</v>
+      </c>
       <c r="G205" s="1"/>
       <c r="H205" s="1"/>
     </row>
@@ -8557,6 +9384,10 @@
         <v>54772184</v>
       </c>
       <c r="D206" s="1"/>
+      <c r="E206">
+        <f t="shared" si="3"/>
+        <v>0.45093691457756802</v>
+      </c>
       <c r="G206" s="1"/>
       <c r="H206" s="1"/>
     </row>
@@ -8568,6 +9399,10 @@
         <v>54772184</v>
       </c>
       <c r="D207" s="1"/>
+      <c r="E207">
+        <f t="shared" si="3"/>
+        <v>0.24573703235095407</v>
+      </c>
       <c r="G207" s="1"/>
       <c r="H207" s="1"/>
     </row>

</xml_diff>